<commit_message>
Added excel file with test history of models
</commit_message>
<xml_diff>
--- a/model_descriptions.xlsx
+++ b/model_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supernova/Dropbox/labwork/APDL_Quality_Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BA33E5-12A5-A149-81FC-8FE11B5DCC90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEECEEA-9C7B-DA4A-9759-2A331D442D55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{48460606-A6B4-F444-925A-76B27474D200}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Model Name</t>
   </si>
@@ -48,16 +48,40 @@
     <t>Raw Code (picture)</t>
   </si>
   <si>
-    <t xml:space="preserve">Preformance </t>
-  </si>
-  <si>
     <t>models/04_20_2:32:26PM/</t>
   </si>
   <si>
     <t>Epoch 10/10, 70/70, 24ms/step - loss: 0.0124 - accuracy: 0.9965 - val_loss: 1.1312 - val_accuracy: 0.8345</t>
   </si>
   <si>
-    <t xml:space="preserve">A preprocessing layer that rescales the layer to a shape of (height, width, 3) </t>
+    <t>Training Details</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/VQoLgxR.png</t>
+  </si>
+  <si>
+    <t>models/04_20_3:59:37PM/</t>
+  </si>
+  <si>
+    <t>The default model from the tutoral</t>
+  </si>
+  <si>
+    <t>Default model with layser.Dropout(0.2)</t>
+  </si>
+  <si>
+    <t>loss: 0.0508 - accuracy: 0.9812 - val_loss: 1.2555 - val_accuracy: 0.8237</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/EYitGMG.png</t>
+  </si>
+  <si>
+    <t>Preformance</t>
+  </si>
+  <si>
+    <t>Worse than row two predicting everything with 11% certanty</t>
   </si>
 </sst>
 </file>
@@ -110,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -124,6 +148,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,51 +468,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988D1FD3-21AE-1641-89BE-4D84FB7AD2DF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="3" width="27.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{0C7C680B-352B-794B-9DB7-7664AFAE6DBB}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{0C7C680B-352B-794B-9DB7-7664AFAE6DBB}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{C2C80F0C-A771-B24C-9259-97B4D84F2624}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{472DFCFB-21E1-F740-9E7A-C37767CAC240}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated some advice on readme
</commit_message>
<xml_diff>
--- a/model_descriptions.xlsx
+++ b/model_descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supernova/Dropbox/labwork/APDL_Quality_Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEECEEA-9C7B-DA4A-9759-2A331D442D55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9345B25B-01FB-6443-8C3B-85F1F5AC1478}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{48460606-A6B4-F444-925A-76B27474D200}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{48460606-A6B4-F444-925A-76B27474D200}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Model Name</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>Worse than row two predicting everything with 11% certanty</t>
+  </si>
+  <si>
+    <t>Mobile Net pretrained model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Better than most models </t>
+  </si>
+  <si>
+    <t xml:space="preserve">change input shape </t>
+  </si>
+  <si>
+    <t xml:space="preserve">try removing rescaling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">greyscale </t>
   </si>
 </sst>
 </file>
@@ -468,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988D1FD3-21AE-1641-89BE-4D84FB7AD2DF}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,6 +552,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{0C7C680B-352B-794B-9DB7-7664AFAE6DBB}"/>

</xml_diff>